<commit_message>
down to a list of 39
</commit_message>
<xml_diff>
--- a/App Store Ratings analysis.xlsx
+++ b/App Store Ratings analysis.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferralme\nss-data-analytics\projects\app-trader-thesaurus-rex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E02BE654-FF1A-4A5F-832E-798075E9100B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE939AE1-C02D-438B-8D2F-D927276D435B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="avg_rating_count_app" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -79,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -731,6 +742,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1AA3-42DD-B3A2-7AD3B083B7AC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -750,6 +766,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1AA3-42DD-B3A2-7AD3B083B7AC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -769,6 +790,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1AA3-42DD-B3A2-7AD3B083B7AC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -788,6 +814,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-1AA3-42DD-B3A2-7AD3B083B7AC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1128,6 +1159,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-91D8-43FD-8A15-46E5BE0CA4EB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1147,6 +1183,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-91D8-43FD-8A15-46E5BE0CA4EB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1166,6 +1207,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-91D8-43FD-8A15-46E5BE0CA4EB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -3078,7 +3124,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>